<commit_message>
Changed to Evidence and EvidenceSet
</commit_message>
<xml_diff>
--- a/image/account.xlsx
+++ b/image/account.xlsx
@@ -827,43 +827,43 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="34.375" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="11.34765625" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="38.45703125" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="4" max="4" width="6.14453125" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="5" max="5" width="4.58203125" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="4.94140625" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="14.70703125" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="12.1875" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="13.0625" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="34.6875" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="11.1328125" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="38.81640625" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="4" max="4" width="5.8984375" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="5" max="5" width="4.69921875" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="5.07421875" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="14.625" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="11.98828125" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="12.74609375" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="115.69140625" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="116.25" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>
-    <col min="15" max="15" width="13.86328125" customWidth="true" bestFit="true"/>
+    <col min="15" max="15" width="13.52734375" customWidth="true" bestFit="true"/>
     <col min="16" max="16" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="17" max="17" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="18" max="18" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="19" max="19" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="20" max="20" width="15.7734375" customWidth="true" bestFit="true"/>
-    <col min="21" max="21" width="16.1328125" customWidth="true" bestFit="true"/>
-    <col min="22" max="22" width="17.40234375" customWidth="true" bestFit="true"/>
-    <col min="23" max="23" width="16.95703125" customWidth="true" bestFit="true"/>
-    <col min="24" max="24" width="61.125" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="45.95703125" customWidth="true" bestFit="true"/>
-    <col min="26" max="26" width="5.8828125" customWidth="true" bestFit="true"/>
-    <col min="27" max="27" width="20.83984375" customWidth="true" bestFit="true"/>
-    <col min="28" max="28" width="18.84375" customWidth="true" bestFit="true"/>
-    <col min="29" max="29" width="15.69921875" customWidth="true" bestFit="true"/>
-    <col min="30" max="30" width="13.12109375" customWidth="true" bestFit="true"/>
-    <col min="31" max="31" width="33.4296875" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="32" max="32" width="9.52734375" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="33" max="33" width="9.890625" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="34" max="34" width="12.71875" customWidth="true" bestFit="true"/>
+    <col min="20" max="20" width="15.7109375" customWidth="true" bestFit="true"/>
+    <col min="21" max="21" width="16.0859375" customWidth="true" bestFit="true"/>
+    <col min="22" max="22" width="17.078125" customWidth="true" bestFit="true"/>
+    <col min="23" max="23" width="16.30859375" customWidth="true" bestFit="true"/>
+    <col min="24" max="24" width="60.79296875" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="45.62109375" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" width="5.69140625" customWidth="true" bestFit="true"/>
+    <col min="27" max="27" width="19.73046875" customWidth="true" bestFit="true"/>
+    <col min="28" max="28" width="17.8203125" customWidth="true" bestFit="true"/>
+    <col min="29" max="29" width="14.984375" customWidth="true" bestFit="true"/>
+    <col min="30" max="30" width="12.30078125" customWidth="true" bestFit="true"/>
+    <col min="31" max="31" width="34.0703125" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="32" max="32" width="9.5" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="33" max="33" width="9.875" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="34" max="34" width="12.21875" customWidth="true" bestFit="true"/>
     <col min="35" max="35" width="100.703125" customWidth="true"/>
-    <col min="36" max="36" width="57.42578125" customWidth="true" bestFit="true"/>
-    <col min="37" max="37" width="33.046875" customWidth="true" bestFit="true"/>
+    <col min="36" max="36" width="58.58984375" customWidth="true" bestFit="true"/>
+    <col min="37" max="37" width="32.84375" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>